<commit_message>
Finalización de metodología, inicio de análisis de requerimientos
</commit_message>
<xml_diff>
--- a/Informe/Images/Gráficos Burn Up - Burn Down.xlsx
+++ b/Informe/Images/Gráficos Burn Up - Burn Down.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPB\Sexto Semestre\Practica-Interna\Proyecto\Informe\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26E2CBE5-E510-45B8-95C5-2FBC4D599106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857ADA7-E79B-407B-94D0-F0D5EE7423AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75E9E56C-E675-4DB3-B11C-17AE4296301D}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{75E9E56C-E675-4DB3-B11C-17AE4296301D}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfica Burn Up" sheetId="1" r:id="rId1"/>
     <sheet name="Gráfica Burn Down" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,24 +26,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Project Total Points</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Cumulative Completed</t>
-  </si>
-  <si>
-    <t>Estimate Trajectory</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Total Hours Estimated By Person Of Work * 3 (40 dias, 2 a 3 horas al día, 3 personas)</t>
   </si>
   <si>
     <t>Versión 0.1</t>
+  </si>
+  <si>
+    <t>horas al dia</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Días totales de trabajo</t>
+  </si>
+  <si>
+    <t>Horas Acumuladas</t>
+  </si>
+  <si>
+    <t>Trayectoria Estimada</t>
+  </si>
+  <si>
+    <t>Horas Estimadas de Trabajo</t>
+  </si>
+  <si>
+    <t>Tareas Completadas</t>
+  </si>
+  <si>
+    <t>Remanente Ideal</t>
+  </si>
+  <si>
+    <t>Tareas Remanentes</t>
+  </si>
+  <si>
+    <t>Esfuerzo Remanente</t>
   </si>
 </sst>
 </file>
@@ -161,49 +179,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1700</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1700</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -224,7 +236,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Project Total Points</c:v>
+                  <c:v>Horas Estimadas de Trabajo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -248,49 +260,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1800</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2200</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2200</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2200</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2200</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -311,7 +317,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cumulative Completed</c:v>
+                  <c:v>Horas Acumuladas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -341,43 +347,37 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>260</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>#N/A</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>#N/A</c:v>
+                  <c:v>585</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>#N/A</c:v>
+                  <c:v>755</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>#N/A</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>#N/A</c:v>
+                  <c:v>935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,7 +398,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Estimate Trajectory</c:v>
+                  <c:v>Trayectoria Estimada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -422,49 +422,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>61.53846153846154</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>157.14285714285714</c:v>
+                  <c:v>123.07692307692308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>314.28571428571428</c:v>
+                  <c:v>184.61538461538461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>471.42857142857144</c:v>
+                  <c:v>246.15384615384616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>628.57142857142856</c:v>
+                  <c:v>307.69230769230768</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>785.71428571428567</c:v>
+                  <c:v>369.23076923076923</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>942.85714285714289</c:v>
+                  <c:v>430.76923076923077</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1100</c:v>
+                  <c:v>492.30769230769232</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1257.1428571428571</c:v>
+                  <c:v>553.84615384615381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1414.2857142857142</c:v>
+                  <c:v>615.38461538461536</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1571.4285714285713</c:v>
+                  <c:v>676.92307692307691</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1728.5714285714287</c:v>
+                  <c:v>738.46153846153845</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1885.7142857142858</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2042.8571428571429</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2200</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -477,7 +471,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -517,7 +510,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-BO"/>
-                  <a:t>Sprints</a:t>
+                  <a:t>Semanas</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -644,13 +637,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="es-BO"/>
-                  <a:t>Total</a:t>
+                  <a:t>Cantidad de Horas Totales</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="es-BO" baseline="0"/>
-                  <a:t> Amount Of Hours</a:t>
-                </a:r>
-                <a:endParaRPr lang="es-BO"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -801,7 +789,762 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-BO"/>
+              <a:t>Gráfico</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-BO" baseline="0"/>
+              <a:t> Burn-Down</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-BO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.8943861133159146E-2"/>
+          <c:y val="0.17147480351363847"/>
+          <c:w val="0.64766964911828462"/>
+          <c:h val="0.71257520876951363"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfica Burn Down'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tareas Completadas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfica Burn Down'!$F$2:$F$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-45B3-4DFA-846E-72ED8CBA6FDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="446283888"/>
+        <c:axId val="446282576"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfica Burn Down'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remanente Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfica Burn Down'!$B$2:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>738.46153846153845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>676.92307692307691</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>615.38461538461536</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>553.84615384615381</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>492.30769230769232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>430.76923076923077</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>369.23076923076923</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>307.69230769230768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>246.15384615384616</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>184.61538461538461</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>123.07692307692308</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>61.53846153846154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-45B3-4DFA-846E-72ED8CBA6FDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfica Burn Down'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Esfuerzo Remanente</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfica Burn Down'!$E$2:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>935</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>915</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-45B3-4DFA-846E-72ED8CBA6FDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="582463416"/>
+        <c:axId val="582462104"/>
+      </c:lineChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Gráfica Burn Down'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tareas Remanentes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Gráfica Burn Down'!$D$2:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-45B3-4DFA-846E-72ED8CBA6FDA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="446283888"/>
+        <c:axId val="446282576"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="582463416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-BO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="582462104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="582462104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-BO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="582463416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="446282576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-BO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446283888"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="446283888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="446282576"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.74560524564783603"/>
+          <c:y val="0.27907836779918083"/>
+          <c:w val="0.23325433228804335"/>
+          <c:h val="0.42533380559264"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-BO"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-BO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1357,6 +2100,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1378,6 +2624,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF250440-C740-4DE6-8911-A12AE8170A99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>308412</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>117781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>268014</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>42040</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0857D259-F2B4-4396-AA24-02BD28D89F55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1695,40 +2982,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCD22C4-406B-4FC3-8D6B-7C124FB77209}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B2">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1737,320 +3026,347 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <f>(B2*A17)/13</f>
+        <v>61.53846153846154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B3">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3">
+        <f>C3+D2</f>
         <v>20</v>
       </c>
       <c r="E3">
-        <f>2200/14</f>
-        <v>157.14285714285714</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E14" si="0">(B3*A18)/13</f>
+        <v>123.07692307692308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B4">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <f t="shared" ref="D4:D14" si="1">C4+D3</f>
+        <v>35</v>
       </c>
       <c r="E4">
-        <f>2200/7</f>
-        <v>314.28571428571428</v>
-      </c>
-      <c r="G4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>184.61538461538461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B5">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="E5">
-        <f>2200*3/14</f>
-        <v>471.42857142857144</v>
-      </c>
-      <c r="G5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>246.15384615384616</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B6">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>65</v>
       </c>
       <c r="E6">
-        <f>2200*4/14</f>
-        <v>628.57142857142856</v>
-      </c>
-      <c r="G6">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>307.69230769230768</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B7">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>75</v>
       </c>
       <c r="E7">
-        <f>2200*5/14</f>
-        <v>785.71428571428567</v>
-      </c>
-      <c r="G7">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>369.23076923076923</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1700</v>
+        <v>600</v>
       </c>
       <c r="B8">
-        <v>1800</v>
+        <v>800</v>
       </c>
       <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>430.76923076923077</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>600</v>
+      </c>
+      <c r="B9">
+        <v>800</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>492.30769230769232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>600</v>
+      </c>
+      <c r="B10">
+        <v>800</v>
+      </c>
+      <c r="C10">
+        <v>170</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>553.84615384615381</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>600</v>
+      </c>
+      <c r="B11">
+        <v>800</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>615.38461538461536</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>600</v>
+      </c>
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12">
+        <v>180</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>585</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>676.92307692307691</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>600</v>
+      </c>
+      <c r="B13">
+        <v>800</v>
+      </c>
+      <c r="C13">
+        <v>170</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>755</v>
+      </c>
+      <c r="E13">
+        <f>(B13*A28)/13</f>
+        <v>738.46153846153845</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>600</v>
+      </c>
+      <c r="B14">
+        <v>800</v>
+      </c>
+      <c r="C14">
+        <v>180</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>935</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>91</v>
+      </c>
+      <c r="G22">
+        <f>D22*E22*F22</f>
+        <v>819</v>
+      </c>
+      <c r="J22">
+        <f>D14/G22</f>
+        <v>1.1416361416361416</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <f>D23*E23*F23</f>
+        <v>840</v>
+      </c>
+      <c r="J23">
+        <f>D14/G23</f>
+        <v>1.1130952380952381</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>10</v>
       </c>
-      <c r="D8">
-        <v>70</v>
-      </c>
-      <c r="E8">
-        <f>2200*6/14</f>
-        <v>942.85714285714289</v>
-      </c>
-      <c r="G8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1700</v>
-      </c>
-      <c r="B9">
-        <v>1800</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>80</v>
-      </c>
-      <c r="E9">
-        <f>2200/2</f>
-        <v>1100</v>
-      </c>
-      <c r="G9">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1700</v>
-      </c>
-      <c r="B10">
-        <v>1800</v>
-      </c>
-      <c r="C10">
-        <v>180</v>
-      </c>
-      <c r="D10">
-        <v>260</v>
-      </c>
-      <c r="E10">
-        <f>2200*8/14</f>
-        <v>1257.1428571428571</v>
-      </c>
-      <c r="G10">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1700</v>
-      </c>
-      <c r="B11">
-        <v>1800</v>
-      </c>
-      <c r="C11" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D11" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E11">
-        <f>2200*9/14</f>
-        <v>1414.2857142857142</v>
-      </c>
-      <c r="G11">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1700</v>
-      </c>
-      <c r="B12">
-        <v>2200</v>
-      </c>
-      <c r="C12" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D12" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E12">
-        <f>2200*10/14</f>
-        <v>1571.4285714285713</v>
-      </c>
-      <c r="G12">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1700</v>
-      </c>
-      <c r="B13">
-        <v>2200</v>
-      </c>
-      <c r="C13" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D13" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E13">
-        <f>2200*11/14</f>
-        <v>1728.5714285714287</v>
-      </c>
-      <c r="G13">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1700</v>
-      </c>
-      <c r="B14">
-        <v>2200</v>
-      </c>
-      <c r="C14" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D14" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E14">
-        <f>2200*12/14</f>
-        <v>1885.7142857142858</v>
-      </c>
-      <c r="G14">
-        <v>1650</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1700</v>
-      </c>
-      <c r="B15">
-        <v>2200</v>
-      </c>
-      <c r="C15" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D15" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E15">
-        <f>2200*13/14</f>
-        <v>2042.8571428571429</v>
-      </c>
-      <c r="G15">
-        <v>2010</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1700</v>
-      </c>
-      <c r="B16">
-        <v>2200</v>
-      </c>
-      <c r="C16" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D16" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E16">
-        <v>2200</v>
-      </c>
-      <c r="G16">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>4</v>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2061,12 +3377,466 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078A1191-EA41-4F51-81EE-AEBA727CAE41}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>600</v>
+      </c>
+      <c r="B2">
+        <f>B17*A29/13</f>
+        <v>800</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D14" si="0">SUM(F2:F14)-F2</f>
+        <v>38</v>
+      </c>
+      <c r="E2">
+        <f>SUM(C2:C14)-C2</f>
+        <v>935</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>600</v>
+      </c>
+      <c r="B3">
+        <f>B17*A30/13</f>
+        <v>738.46153846153845</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="1">SUM(C3:C15)-C3</f>
+        <v>915</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>600</v>
+      </c>
+      <c r="B4">
+        <f>B17*A31/13</f>
+        <v>676.92307692307691</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>600</v>
+      </c>
+      <c r="B5">
+        <f>B17*A32/13</f>
+        <v>615.38461538461536</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>890</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>600</v>
+      </c>
+      <c r="B6">
+        <f>B17*A33/13</f>
+        <v>553.84615384615381</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>600</v>
+      </c>
+      <c r="B7">
+        <f>B17*A34/13</f>
+        <v>492.30769230769232</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>860</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>600</v>
+      </c>
+      <c r="B8">
+        <f>B17*A35/13</f>
+        <v>430.76923076923077</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>855</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>600</v>
+      </c>
+      <c r="B9">
+        <f>B17*A36/13</f>
+        <v>369.23076923076923</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>850</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>600</v>
+      </c>
+      <c r="B10">
+        <f>B17*A37/13</f>
+        <v>307.69230769230768</v>
+      </c>
+      <c r="C10">
+        <v>170</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>680</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>600</v>
+      </c>
+      <c r="B11">
+        <f>B17*A38/13</f>
+        <v>246.15384615384616</v>
+      </c>
+      <c r="C11">
+        <v>150</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>530</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>600</v>
+      </c>
+      <c r="B12">
+        <f>B17*A39/13</f>
+        <v>184.61538461538461</v>
+      </c>
+      <c r="C12">
+        <v>180</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>600</v>
+      </c>
+      <c r="B13">
+        <f>B17*A40/13</f>
+        <v>123.07692307692308</v>
+      </c>
+      <c r="C13">
+        <v>170</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>600</v>
+      </c>
+      <c r="B14">
+        <f>B17*A41/13</f>
+        <v>61.53846153846154</v>
+      </c>
+      <c r="C14">
+        <v>180</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redacción de Diseño, revisión, redacción y correción en varios lugares
</commit_message>
<xml_diff>
--- a/Informe/Images/Gráficos Burn Up - Burn Down.xlsx
+++ b/Informe/Images/Gráficos Burn Up - Burn Down.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPB\Sexto Semestre\Practica-Interna\Proyecto\Informe\Images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F857ADA7-E79B-407B-94D0-F0D5EE7423AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F610F1-8828-4514-BB5E-6EB5E7C9AA20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{75E9E56C-E675-4DB3-B11C-17AE4296301D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75E9E56C-E675-4DB3-B11C-17AE4296301D}"/>
   </bookViews>
   <sheets>
     <sheet name="Gráfica Burn Up" sheetId="1" r:id="rId1"/>
@@ -130,7 +130,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-BO"/>
+              <a:t>Gráfico</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-BO" baseline="0"/>
+              <a:t> Burn-Up</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-BO"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-BO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -139,8 +199,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.12238735783027122"/>
           <c:y val="0.10389327652847279"/>
-          <c:w val="0.87753018372703417"/>
-          <c:h val="0.54316873464530424"/>
+          <c:w val="0.64363042607071907"/>
+          <c:h val="0.73336581495592346"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -365,19 +425,19 @@
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>255</c:v>
+                  <c:v>195</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>405</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>585</c:v>
+                  <c:v>440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>755</c:v>
+                  <c:v>580</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>935</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -519,8 +579,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.50508289588801403"/>
-              <c:y val="0.74573963545748678"/>
+              <c:x val="0.3599783426130404"/>
+              <c:y val="0.91903056999922794"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -716,6 +776,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.69322430743257635"/>
+          <c:y val="0.31159128001554859"/>
+          <c:w val="0.28276447165355001"/>
+          <c:h val="0.22770882089047564"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -869,10 +939,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8943861133159146E-2"/>
+          <c:x val="9.7740012285916514E-2"/>
           <c:y val="0.17147480351363847"/>
-          <c:w val="0.64766964911828462"/>
-          <c:h val="0.71257520876951363"/>
+          <c:w val="0.61887339331641955"/>
+          <c:h val="0.68045146658344824"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1086,37 +1156,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>935</c:v>
+                  <c:v>825</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>915</c:v>
+                  <c:v>805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>900</c:v>
+                  <c:v>790</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>890</c:v>
+                  <c:v>780</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>870</c:v>
+                  <c:v>760</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>860</c:v>
+                  <c:v>750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>855</c:v>
+                  <c:v>745</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>850</c:v>
+                  <c:v>740</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>680</c:v>
+                  <c:v>620</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>530</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>350</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>180</c:v>
@@ -2613,8 +2683,8 @@
       <xdr:rowOff>148327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>536750</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>472966</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>105103</xdr:rowOff>
     </xdr:to>
@@ -2649,7 +2719,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>308412</xdr:colOff>
+      <xdr:colOff>32844</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>117781</xdr:rowOff>
     </xdr:from>
@@ -2984,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCD22C4-406B-4FC3-8D6B-7C124FB77209}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,11 +3241,11 @@
         <v>800</v>
       </c>
       <c r="C10">
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>255</v>
+        <v>195</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
@@ -3190,11 +3260,11 @@
         <v>800</v>
       </c>
       <c r="C11">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>405</v>
+        <v>310</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
@@ -3209,11 +3279,11 @@
         <v>800</v>
       </c>
       <c r="C12">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>585</v>
+        <v>440</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
@@ -3228,11 +3298,11 @@
         <v>800</v>
       </c>
       <c r="C13">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>755</v>
+        <v>580</v>
       </c>
       <c r="E13">
         <f>(B13*A28)/13</f>
@@ -3247,11 +3317,11 @@
         <v>800</v>
       </c>
       <c r="C14">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>935</v>
+        <v>750</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
@@ -3314,7 +3384,7 @@
       </c>
       <c r="J22">
         <f>D14/G22</f>
-        <v>1.1416361416361416</v>
+        <v>0.91575091575091572</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3336,7 +3406,7 @@
       </c>
       <c r="J23">
         <f>D14/G23</f>
-        <v>1.1130952380952381</v>
+        <v>0.8928571428571429</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3379,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078A1191-EA41-4F51-81EE-AEBA727CAE41}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3425,7 +3495,7 @@
       </c>
       <c r="E2">
         <f>SUM(C2:C14)-C2</f>
-        <v>935</v>
+        <v>825</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -3448,7 +3518,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E14" si="1">SUM(C3:C15)-C3</f>
-        <v>915</v>
+        <v>805</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3471,7 +3541,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>790</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -3494,7 +3564,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>890</v>
+        <v>780</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -3517,7 +3587,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>870</v>
+        <v>760</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -3540,7 +3610,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>860</v>
+        <v>750</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -3563,7 +3633,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>855</v>
+        <v>745</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -3586,7 +3656,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>850</v>
+        <v>740</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3601,7 +3671,7 @@
         <v>307.69230769230768</v>
       </c>
       <c r="C10">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -3609,7 +3679,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>680</v>
+        <v>620</v>
       </c>
       <c r="F10">
         <v>7</v>
@@ -3624,7 +3694,7 @@
         <v>246.15384615384616</v>
       </c>
       <c r="C11">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -3632,7 +3702,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>530</v>
+        <v>490</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -3647,7 +3717,7 @@
         <v>184.61538461538461</v>
       </c>
       <c r="C12">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -3655,7 +3725,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -3670,7 +3740,7 @@
         <v>123.07692307692308</v>
       </c>
       <c r="C13">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>

</xml_diff>